<commit_message>
Saving the catches and discard fate Excel files for EwE.
</commit_message>
<xml_diff>
--- a/WGOA_source_data/EwE_wgoa_catches_alt_v.xlsx
+++ b/WGOA_source_data/EwE_wgoa_catches_alt_v.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biadias\Documents\WGOA-Ecopath-Rpath\WGOA_source_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C2271D-9837-4D47-A51A-F420D1D9F641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7AA6FE-2E26-4E82-871D-7A7B74A3ACD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{27374A76-405C-49B2-ABB2-B6A016766631}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{27374A76-405C-49B2-ABB2-B6A016766631}"/>
   </bookViews>
   <sheets>
     <sheet name="METADATA" sheetId="4" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="175">
   <si>
     <t>Group name</t>
   </si>
@@ -380,21 +380,6 @@
   </si>
   <si>
     <t>JIG_federal</t>
-  </si>
-  <si>
-    <t>king_state</t>
-  </si>
-  <si>
-    <t>herring_state</t>
-  </si>
-  <si>
-    <t>salmon_state</t>
-  </si>
-  <si>
-    <t>tanner_crab_state</t>
-  </si>
-  <si>
-    <t>lingcod_state</t>
   </si>
   <si>
     <t>Catches:</t>
@@ -591,8 +576,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="0.000000000"/>
-    <numFmt numFmtId="172" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000000"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -647,22 +632,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -1034,7 +1017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4380B128-6D61-416F-A0C1-05CC70C00498}">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -1044,305 +1027,305 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="B1" s="14" t="s">
+      <c r="A1" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="13" t="s">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="11" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="13" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="11" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="11" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="13" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="11" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="13" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="11" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="13" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="11" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="13" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="11" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="13" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="11" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="13" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="11" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="13" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="11" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="13" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="11" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="13" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="11" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="13" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="11" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="13" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="11" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="13" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="11" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="13" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="11" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="13" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="11" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="13" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="11" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="13" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="11" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="13" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="11" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="13" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="11" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="13" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="11" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="13" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="11" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="13" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="11" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="13" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="11" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="13" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+      <c r="B32" s="12" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="13" t="s">
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
+      <c r="B33" s="12" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="13" t="s">
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="11" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="13" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="11" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="13" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="11" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="14" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="14" t="s">
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="13" t="s">
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="11" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="13" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="11" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="13" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="11" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="13" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="11" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="13" t="s">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B43" s="11" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="13" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B44" s="11" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="13" t="s">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B45" s="11" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="13" t="s">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="11" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B42" s="13" t="s">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B47" s="11" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B43" s="13" t="s">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B48" s="11" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B44" s="13" t="s">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="11" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B45" s="13" t="s">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="11" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B46" s="13" t="s">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="11" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B47" s="13" t="s">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" s="11" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B48" s="13" t="s">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" s="11" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" s="13" t="s">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" s="11" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="13" t="s">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55" s="11" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="13" t="s">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56" s="11" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B52" s="13" t="s">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B57" s="10" t="s">
         <v>168</v>
-      </c>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B53" s="13" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B54" s="13" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B55" s="13" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B56" s="13" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B57" s="12" t="s">
-        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -1503,7 +1486,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1526,7 +1509,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1549,7 +1532,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1572,7 +1555,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1595,7 +1578,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1620,11 +1603,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1B61ACA-ED6A-4045-8EF4-52A6AB899584}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:M98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F124" sqref="F124"/>
+      <selection activeCell="C1" sqref="C1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1632,7 +1614,7 @@
     <col min="1" max="1" width="6.5703125" customWidth="1"/>
     <col min="2" max="2" width="23.85546875" customWidth="1"/>
     <col min="3" max="12" width="18.140625" customWidth="1"/>
-    <col min="13" max="13" width="18.140625" style="7" customWidth="1"/>
+    <col min="13" max="13" width="18.140625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1655,32 +1637,32 @@
         <v>111</v>
       </c>
       <c r="H1" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="I1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="J1" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="K1" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="L1" t="s">
-        <v>179</v>
-      </c>
-      <c r="M1" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="M1" s="8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>0</v>
       </c>
       <c r="D2">
@@ -1707,19 +1689,19 @@
       <c r="L2">
         <v>0</v>
       </c>
-      <c r="M2" s="7">
+      <c r="M2" s="6">
         <f>SUM(C2:L2)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>0</v>
       </c>
       <c r="D3">
@@ -1746,19 +1728,19 @@
       <c r="L3">
         <v>0</v>
       </c>
-      <c r="M3" s="7">
+      <c r="M3" s="6">
         <f t="shared" ref="M3:M21" si="0">SUM(C3:L3)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>0</v>
       </c>
       <c r="D4">
@@ -1785,19 +1767,19 @@
       <c r="L4">
         <v>0</v>
       </c>
-      <c r="M4" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M4" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>0</v>
       </c>
       <c r="D5">
@@ -1824,19 +1806,19 @@
       <c r="L5">
         <v>0</v>
       </c>
-      <c r="M5" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M5" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>0</v>
       </c>
       <c r="D6">
@@ -1863,19 +1845,19 @@
       <c r="L6">
         <v>0</v>
       </c>
-      <c r="M6" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M6" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>8.5700000000000006E-8</v>
       </c>
       <c r="D7">
@@ -1902,19 +1884,19 @@
       <c r="L7">
         <v>0</v>
       </c>
-      <c r="M7" s="7">
+      <c r="M7" s="6">
         <f t="shared" si="0"/>
         <v>8.5700000000000006E-8</v>
       </c>
     </row>
-    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>1.29E-7</v>
       </c>
       <c r="D8">
@@ -1941,19 +1923,19 @@
       <c r="L8">
         <v>0</v>
       </c>
-      <c r="M8" s="7">
+      <c r="M8" s="6">
         <f t="shared" si="0"/>
         <v>1.29E-7</v>
       </c>
     </row>
-    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>0</v>
       </c>
       <c r="D9">
@@ -1980,19 +1962,19 @@
       <c r="L9">
         <v>0</v>
       </c>
-      <c r="M9" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M9" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>5.09475E-5</v>
       </c>
       <c r="D10">
@@ -2019,19 +2001,19 @@
       <c r="L10">
         <v>0</v>
       </c>
-      <c r="M10" s="7">
+      <c r="M10" s="6">
         <f t="shared" si="0"/>
         <v>5.09475E-5</v>
       </c>
     </row>
-    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>0</v>
       </c>
       <c r="D11">
@@ -2058,19 +2040,19 @@
       <c r="L11">
         <v>0</v>
       </c>
-      <c r="M11" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M11" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>4.1699999999999997E-5</v>
       </c>
       <c r="D12">
@@ -2097,19 +2079,19 @@
       <c r="L12">
         <v>0</v>
       </c>
-      <c r="M12" s="7">
+      <c r="M12" s="6">
         <f t="shared" si="0"/>
         <v>4.1699999999999997E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>5.2330000000000002E-5</v>
       </c>
       <c r="D13">
@@ -2136,19 +2118,19 @@
       <c r="L13">
         <v>0</v>
       </c>
-      <c r="M13" s="7">
+      <c r="M13" s="6">
         <f t="shared" si="0"/>
         <v>5.2330000000000002E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>3.62E-8</v>
       </c>
       <c r="D14">
@@ -2175,19 +2157,19 @@
       <c r="L14">
         <v>0</v>
       </c>
-      <c r="M14" s="7">
+      <c r="M14" s="6">
         <f t="shared" si="0"/>
         <v>3.62E-8</v>
       </c>
     </row>
-    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <v>0</v>
       </c>
       <c r="D15">
@@ -2214,19 +2196,19 @@
       <c r="L15">
         <v>0</v>
       </c>
-      <c r="M15" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M15" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="3">
         <v>0</v>
       </c>
       <c r="D16">
@@ -2253,19 +2235,19 @@
       <c r="L16">
         <v>0</v>
       </c>
-      <c r="M16" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M16" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <v>0</v>
       </c>
       <c r="D17">
@@ -2292,19 +2274,19 @@
       <c r="L17">
         <v>0</v>
       </c>
-      <c r="M17" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M17" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="3">
         <v>0</v>
       </c>
       <c r="D18">
@@ -2331,19 +2313,19 @@
       <c r="L18">
         <v>0</v>
       </c>
-      <c r="M18" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M18" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="3">
         <v>2.8465700000000001E-3</v>
       </c>
       <c r="D19">
@@ -2373,19 +2355,19 @@
       <c r="L19">
         <v>0.38997674840673202</v>
       </c>
-      <c r="M19" s="7">
+      <c r="M19" s="6">
         <f t="shared" si="0"/>
         <v>0.39284166606263776</v>
       </c>
     </row>
-    <row r="20" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="3">
         <v>0</v>
       </c>
       <c r="D20">
@@ -2412,19 +2394,19 @@
       <c r="L20">
         <v>0</v>
       </c>
-      <c r="M20" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M20" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="3">
         <v>0</v>
       </c>
       <c r="D21">
@@ -2451,25 +2433,25 @@
       <c r="L21">
         <v>0</v>
       </c>
-      <c r="M21" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M21" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="4"/>
-    </row>
-    <row r="23" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="4">
         <v>6.8999999999999997E-5</v>
       </c>
       <c r="D23">
@@ -2496,19 +2478,19 @@
       <c r="L23">
         <v>1.4370333120358033E-2</v>
       </c>
-      <c r="M23" s="7">
+      <c r="M23" s="6">
         <f>SUM(C23:L23)</f>
         <v>1.4451313935508244E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="3">
         <v>0</v>
       </c>
       <c r="D24">
@@ -2535,19 +2517,19 @@
       <c r="L24">
         <v>0</v>
       </c>
-      <c r="M24" s="7">
+      <c r="M24" s="6">
         <f t="shared" ref="M24:M87" si="1">SUM(C24:L24)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="3">
         <v>0</v>
       </c>
       <c r="D25">
@@ -2577,19 +2559,19 @@
       <c r="L25">
         <v>0</v>
       </c>
-      <c r="M25" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M25" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26" s="3">
         <v>0</v>
       </c>
       <c r="D26">
@@ -2616,19 +2598,19 @@
       <c r="L26">
         <v>0</v>
       </c>
-      <c r="M26" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M26" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="4">
         <v>6.7199999999999994E-5</v>
       </c>
       <c r="D27">
@@ -2658,19 +2640,19 @@
       <c r="L27">
         <v>0</v>
       </c>
-      <c r="M27" s="7">
+      <c r="M27" s="6">
         <f t="shared" si="1"/>
         <v>4.5721117986190701E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="3">
         <v>0</v>
       </c>
       <c r="D28">
@@ -2697,19 +2679,19 @@
       <c r="L28">
         <v>0</v>
       </c>
-      <c r="M28" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M28" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="4">
         <v>9.8900000000000005E-8</v>
       </c>
       <c r="D29">
@@ -2739,19 +2721,19 @@
       <c r="L29">
         <v>0</v>
       </c>
-      <c r="M29" s="7">
+      <c r="M29" s="6">
         <f t="shared" si="1"/>
         <v>9.8900000000000005E-8</v>
       </c>
     </row>
-    <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="4">
         <v>8.1800000000000005E-8</v>
       </c>
       <c r="D30">
@@ -2778,19 +2760,19 @@
       <c r="L30">
         <v>0</v>
       </c>
-      <c r="M30" s="7">
+      <c r="M30" s="6">
         <f t="shared" si="1"/>
         <v>8.1800000000000005E-8</v>
       </c>
     </row>
-    <row r="31" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C31" s="3">
         <v>0</v>
       </c>
       <c r="D31">
@@ -2817,19 +2799,19 @@
       <c r="L31">
         <v>0</v>
       </c>
-      <c r="M31" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M31" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
       <c r="B32" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C32" s="4">
         <v>7.1699999999999997E-7</v>
       </c>
       <c r="D32">
@@ -2859,31 +2841,31 @@
       <c r="L32">
         <v>0</v>
       </c>
-      <c r="M32" s="7">
+      <c r="M32" s="6">
         <f t="shared" si="1"/>
         <v>7.1699999999999997E-7</v>
       </c>
     </row>
-    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
       <c r="B33" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="4">
-        <v>0</v>
-      </c>
-      <c r="D33" s="6">
+      <c r="C33" s="3">
+        <v>0</v>
+      </c>
+      <c r="D33" s="5">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="E33" s="6">
+      <c r="E33" s="5">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="F33">
         <v>0</v>
       </c>
-      <c r="G33" s="6">
+      <c r="G33" s="5">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="H33">
@@ -2901,19 +2883,19 @@
       <c r="L33" s="1">
         <v>0</v>
       </c>
-      <c r="M33" s="7">
+      <c r="M33" s="6">
         <f t="shared" si="1"/>
         <v>3.0000000000000004E-5</v>
       </c>
     </row>
-    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
       <c r="B34" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C34" s="3">
         <v>0</v>
       </c>
       <c r="D34">
@@ -2943,25 +2925,25 @@
       <c r="L34" s="1">
         <v>0</v>
       </c>
-      <c r="M34" s="7">
+      <c r="M34" s="6">
         <f t="shared" si="1"/>
         <v>1.0883858592630772E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="4"/>
-    </row>
-    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C35" s="3"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>33</v>
       </c>
       <c r="B36" t="s">
         <v>37</v>
       </c>
-      <c r="C36" s="4">
+      <c r="C36" s="3">
         <v>5.8887999999999996E-4</v>
       </c>
       <c r="D36">
@@ -2991,19 +2973,19 @@
       <c r="L36">
         <v>0</v>
       </c>
-      <c r="M36" s="7">
+      <c r="M36" s="6">
         <f t="shared" si="1"/>
         <v>5.8736482837143432E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>34</v>
       </c>
       <c r="B37" t="s">
         <v>38</v>
       </c>
-      <c r="C37" s="4">
+      <c r="C37" s="3">
         <v>0</v>
       </c>
       <c r="D37">
@@ -3033,25 +3015,25 @@
       <c r="L37">
         <v>0</v>
       </c>
-      <c r="M37" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M37" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>39</v>
       </c>
-      <c r="C38" s="4"/>
-    </row>
-    <row r="39" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C38" s="3"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>35</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C39" s="4">
         <v>2.9400000000000001E-7</v>
       </c>
       <c r="D39">
@@ -3081,19 +3063,19 @@
       <c r="L39" s="1">
         <v>0</v>
       </c>
-      <c r="M39" s="7">
+      <c r="M39" s="6">
         <f t="shared" si="1"/>
         <v>2.45029760958758E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>36</v>
       </c>
       <c r="B40" t="s">
         <v>41</v>
       </c>
-      <c r="C40" s="4">
+      <c r="C40" s="3">
         <v>0</v>
       </c>
       <c r="D40">
@@ -3120,25 +3102,25 @@
       <c r="L40">
         <v>0</v>
       </c>
-      <c r="M40" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M40" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>42</v>
       </c>
-      <c r="C41" s="4"/>
-    </row>
-    <row r="42" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C41" s="3"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>37</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C42" s="4">
         <v>8.1900000000000001E-7</v>
       </c>
       <c r="D42">
@@ -3168,19 +3150,19 @@
       <c r="L42">
         <v>0</v>
       </c>
-      <c r="M42" s="7">
+      <c r="M42" s="6">
         <f t="shared" si="1"/>
         <v>9.7075797321807267E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>38</v>
       </c>
       <c r="B43" t="s">
         <v>44</v>
       </c>
-      <c r="C43" s="4">
+      <c r="C43" s="3">
         <v>0</v>
       </c>
       <c r="D43">
@@ -3210,25 +3192,25 @@
       <c r="L43">
         <v>0</v>
       </c>
-      <c r="M43" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M43" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>45</v>
       </c>
-      <c r="C44" s="4"/>
-    </row>
-    <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C44" s="3"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>39</v>
       </c>
       <c r="B45" t="s">
         <v>46</v>
       </c>
-      <c r="C45" s="4">
+      <c r="C45" s="3">
         <v>0</v>
       </c>
       <c r="D45">
@@ -3258,19 +3240,19 @@
       <c r="L45">
         <v>0</v>
       </c>
-      <c r="M45" s="7">
+      <c r="M45" s="6">
         <f t="shared" si="1"/>
         <v>1.4518621278788937E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>40</v>
       </c>
       <c r="B46" t="s">
         <v>47</v>
       </c>
-      <c r="C46" s="4">
+      <c r="C46" s="3">
         <v>0</v>
       </c>
       <c r="D46">
@@ -3297,19 +3279,19 @@
       <c r="L46">
         <v>0</v>
       </c>
-      <c r="M46" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M46" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>41</v>
       </c>
       <c r="B47" t="s">
         <v>48</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C47" s="4">
         <v>2.1100000000000001E-5</v>
       </c>
       <c r="D47">
@@ -3339,25 +3321,25 @@
       <c r="L47" s="1">
         <v>0</v>
       </c>
-      <c r="M47" s="7">
+      <c r="M47" s="6">
         <f t="shared" si="1"/>
         <v>4.9684747620029328E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>42</v>
       </c>
       <c r="B48" t="s">
         <v>49</v>
       </c>
-      <c r="C48" s="4">
-        <v>0</v>
-      </c>
-      <c r="D48" s="7">
+      <c r="C48" s="3">
+        <v>0</v>
+      </c>
+      <c r="D48" s="6">
         <v>8.2442741588540259E-5</v>
       </c>
-      <c r="E48" s="7">
+      <c r="E48" s="6">
         <v>2.9773607247975672E-2</v>
       </c>
       <c r="F48">
@@ -3366,32 +3348,32 @@
       <c r="G48">
         <v>0</v>
       </c>
-      <c r="H48" s="7">
+      <c r="H48" s="6">
         <v>1.4413301245053677E-6</v>
       </c>
-      <c r="I48" s="7">
+      <c r="I48" s="6">
         <v>9.9187695729277166E-3</v>
       </c>
       <c r="L48" s="1"/>
-      <c r="M48" s="7">
+      <c r="M48" s="6">
         <f t="shared" si="1"/>
         <v>3.9776260892616433E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>50</v>
       </c>
-      <c r="C49" s="4"/>
-    </row>
-    <row r="50" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C49" s="3"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>43</v>
       </c>
       <c r="B50" t="s">
         <v>51</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C50" s="4">
         <v>6.9362000000000004E-5</v>
       </c>
       <c r="D50">
@@ -3421,19 +3403,19 @@
       <c r="L50" s="1">
         <v>0</v>
       </c>
-      <c r="M50" s="7">
+      <c r="M50" s="6">
         <f t="shared" si="1"/>
         <v>1.3869776651122306E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>44</v>
       </c>
       <c r="B51" t="s">
         <v>52</v>
       </c>
-      <c r="C51" s="4">
+      <c r="C51" s="3">
         <v>0</v>
       </c>
       <c r="D51">
@@ -3463,19 +3445,19 @@
       <c r="L51">
         <v>0</v>
       </c>
-      <c r="M51" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M51" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>45</v>
       </c>
       <c r="B52" t="s">
         <v>53</v>
       </c>
-      <c r="C52" s="4">
+      <c r="C52" s="3">
         <v>0</v>
       </c>
       <c r="D52">
@@ -3505,19 +3487,19 @@
       <c r="L52" s="1">
         <v>0</v>
       </c>
-      <c r="M52" s="7">
+      <c r="M52" s="6">
         <f t="shared" si="1"/>
         <v>3.7790705992242005E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>46</v>
       </c>
       <c r="B53" t="s">
         <v>54</v>
       </c>
-      <c r="C53" s="5">
+      <c r="C53" s="4">
         <v>6.3600000000000001E-5</v>
       </c>
       <c r="D53">
@@ -3547,19 +3529,19 @@
       <c r="L53" s="1">
         <v>0</v>
       </c>
-      <c r="M53" s="7">
+      <c r="M53" s="6">
         <f t="shared" si="1"/>
         <v>1.7103539955757928E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>47</v>
       </c>
       <c r="B54" t="s">
         <v>55</v>
       </c>
-      <c r="C54" s="4">
+      <c r="C54" s="3">
         <v>0</v>
       </c>
       <c r="D54">
@@ -3589,19 +3571,19 @@
       <c r="L54">
         <v>0</v>
       </c>
-      <c r="M54" s="7">
+      <c r="M54" s="6">
         <f t="shared" si="1"/>
         <v>7.5829687628463189E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>48</v>
       </c>
       <c r="B55" t="s">
         <v>56</v>
       </c>
-      <c r="C55" s="4">
+      <c r="C55" s="3">
         <v>0</v>
       </c>
       <c r="D55">
@@ -3631,25 +3613,25 @@
       <c r="L55" s="1">
         <v>0</v>
       </c>
-      <c r="M55" s="7">
+      <c r="M55" s="6">
         <f t="shared" si="1"/>
         <v>6.2421849771477486E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>57</v>
       </c>
-      <c r="C56" s="4"/>
-    </row>
-    <row r="57" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C56" s="3"/>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>49</v>
       </c>
       <c r="B57" t="s">
         <v>58</v>
       </c>
-      <c r="C57" s="5">
+      <c r="C57" s="4">
         <v>4.0200000000000001E-5</v>
       </c>
       <c r="D57">
@@ -3679,19 +3661,19 @@
       <c r="L57" s="1">
         <v>0</v>
       </c>
-      <c r="M57" s="7">
+      <c r="M57" s="6">
         <f t="shared" si="1"/>
         <v>8.050419097794001E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>50</v>
       </c>
       <c r="B58" t="s">
         <v>59</v>
       </c>
-      <c r="C58" s="4">
+      <c r="C58" s="3">
         <v>0</v>
       </c>
       <c r="D58">
@@ -3721,25 +3703,25 @@
       <c r="L58">
         <v>0</v>
       </c>
-      <c r="M58" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M58" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>60</v>
       </c>
-      <c r="C59" s="4"/>
-    </row>
-    <row r="60" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C59" s="3"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>51</v>
       </c>
       <c r="B60" t="s">
         <v>61</v>
       </c>
-      <c r="C60" s="4">
+      <c r="C60" s="3">
         <v>1.2976700000000001E-4</v>
       </c>
       <c r="D60">
@@ -3769,19 +3751,19 @@
       <c r="L60">
         <v>4.664383861157139E-4</v>
       </c>
-      <c r="M60" s="7">
+      <c r="M60" s="6">
         <f t="shared" si="1"/>
         <v>0.5633303491952556</v>
       </c>
     </row>
-    <row r="61" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>52</v>
       </c>
       <c r="B61" t="s">
         <v>62</v>
       </c>
-      <c r="C61" s="4">
+      <c r="C61" s="3">
         <v>0</v>
       </c>
       <c r="D61">
@@ -3811,7 +3793,7 @@
       <c r="L61">
         <v>0</v>
       </c>
-      <c r="M61" s="7">
+      <c r="M61" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3820,7 +3802,7 @@
       <c r="B62" t="s">
         <v>63</v>
       </c>
-      <c r="C62" s="4"/>
+      <c r="C62" s="3"/>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63">
@@ -3829,7 +3811,7 @@
       <c r="B63" t="s">
         <v>64</v>
       </c>
-      <c r="C63" s="5">
+      <c r="C63" s="4">
         <v>7.9500000000000001E-7</v>
       </c>
       <c r="D63">
@@ -3859,7 +3841,7 @@
       <c r="L63">
         <v>1.0670866323918399E-5</v>
       </c>
-      <c r="M63" s="7">
+      <c r="M63" s="6">
         <f t="shared" si="1"/>
         <v>0.7433488082858648</v>
       </c>
@@ -3871,7 +3853,7 @@
       <c r="B64" t="s">
         <v>65</v>
       </c>
-      <c r="C64" s="4">
+      <c r="C64" s="3">
         <v>0</v>
       </c>
       <c r="D64">
@@ -3901,19 +3883,19 @@
       <c r="L64">
         <v>0</v>
       </c>
-      <c r="M64" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M64" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>55</v>
       </c>
       <c r="B65" t="s">
         <v>66</v>
       </c>
-      <c r="C65" s="4">
+      <c r="C65" s="3">
         <v>0</v>
       </c>
       <c r="D65">
@@ -3943,19 +3925,19 @@
       <c r="L65">
         <v>0</v>
       </c>
-      <c r="M65" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M65" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>56</v>
       </c>
       <c r="B66" t="s">
         <v>67</v>
       </c>
-      <c r="C66" s="4">
+      <c r="C66" s="3">
         <v>0</v>
       </c>
       <c r="D66">
@@ -3985,19 +3967,19 @@
       <c r="L66">
         <v>0</v>
       </c>
-      <c r="M66" s="7">
+      <c r="M66" s="6">
         <f t="shared" si="1"/>
         <v>1.0699718687163417E-4</v>
       </c>
     </row>
-    <row r="67" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>57</v>
       </c>
-      <c r="B67" s="6" t="s">
+      <c r="B67" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C67" s="4">
+      <c r="C67" s="3">
         <v>0</v>
       </c>
       <c r="D67">
@@ -4027,19 +4009,19 @@
       <c r="L67">
         <v>0</v>
       </c>
-      <c r="M67" s="7">
+      <c r="M67" s="6">
         <f t="shared" si="1"/>
         <v>3.0531832696537149E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>58</v>
       </c>
       <c r="B68" t="s">
         <v>69</v>
       </c>
-      <c r="C68" s="4">
+      <c r="C68" s="3">
         <v>0</v>
       </c>
       <c r="D68">
@@ -4069,19 +4051,19 @@
       <c r="L68">
         <v>0</v>
       </c>
-      <c r="M68" s="7">
+      <c r="M68" s="6">
         <f t="shared" si="1"/>
         <v>1.8271106977695779E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>59</v>
       </c>
       <c r="B69" t="s">
         <v>70</v>
       </c>
-      <c r="C69" s="4">
+      <c r="C69" s="3">
         <v>0</v>
       </c>
       <c r="D69">
@@ -4111,19 +4093,19 @@
       <c r="L69" s="1">
         <v>0</v>
       </c>
-      <c r="M69" s="7">
+      <c r="M69" s="6">
         <f t="shared" si="1"/>
         <v>1.0048460303873177E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>60</v>
       </c>
       <c r="B70" t="s">
         <v>71</v>
       </c>
-      <c r="C70" s="4">
+      <c r="C70" s="3">
         <v>0</v>
       </c>
       <c r="D70">
@@ -4153,19 +4135,19 @@
       <c r="L70">
         <v>0</v>
       </c>
-      <c r="M70" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M70" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>61</v>
       </c>
       <c r="B71" t="s">
         <v>72</v>
       </c>
-      <c r="C71" s="4">
+      <c r="C71" s="3">
         <v>0</v>
       </c>
       <c r="D71">
@@ -4195,19 +4177,19 @@
       <c r="L71" s="1">
         <v>0</v>
       </c>
-      <c r="M71" s="7">
+      <c r="M71" s="6">
         <f t="shared" si="1"/>
         <v>1.1293559263219022E-4</v>
       </c>
     </row>
-    <row r="72" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>62</v>
       </c>
       <c r="B72" t="s">
         <v>73</v>
       </c>
-      <c r="C72" s="4">
+      <c r="C72" s="3">
         <v>0</v>
       </c>
       <c r="D72">
@@ -4237,19 +4219,19 @@
       <c r="L72" s="1">
         <v>0</v>
       </c>
-      <c r="M72" s="7">
+      <c r="M72" s="6">
         <f t="shared" si="1"/>
         <v>3.3592716693430538E-4</v>
       </c>
     </row>
-    <row r="73" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>63</v>
       </c>
       <c r="B73" t="s">
         <v>74</v>
       </c>
-      <c r="C73" s="5">
+      <c r="C73" s="4">
         <v>9.3332999999999996E-5</v>
       </c>
       <c r="D73">
@@ -4279,19 +4261,19 @@
       <c r="L73">
         <v>0</v>
       </c>
-      <c r="M73" s="7">
+      <c r="M73" s="6">
         <f t="shared" si="1"/>
         <v>4.7123143171074544E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>64</v>
       </c>
       <c r="B74" t="s">
         <v>75</v>
       </c>
-      <c r="C74" s="5">
+      <c r="C74" s="4">
         <v>6.0300000000000002E-5</v>
       </c>
       <c r="D74">
@@ -4321,19 +4303,19 @@
       <c r="L74">
         <v>0</v>
       </c>
-      <c r="M74" s="7">
+      <c r="M74" s="6">
         <f>SUM(C74:L74)</f>
         <v>2.231210360822765E-4</v>
       </c>
     </row>
-    <row r="75" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>65</v>
       </c>
       <c r="B75" t="s">
         <v>76</v>
       </c>
-      <c r="C75" s="5">
+      <c r="C75" s="4">
         <v>6.1299999999999999E-5</v>
       </c>
       <c r="D75">
@@ -4363,19 +4345,19 @@
       <c r="L75">
         <v>0</v>
       </c>
-      <c r="M75" s="7">
+      <c r="M75" s="6">
         <f t="shared" si="1"/>
         <v>6.1299999999999999E-5</v>
       </c>
     </row>
-    <row r="76" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>66</v>
       </c>
       <c r="B76" t="s">
         <v>77</v>
       </c>
-      <c r="C76" s="4">
+      <c r="C76" s="3">
         <v>0</v>
       </c>
       <c r="D76">
@@ -4405,19 +4387,19 @@
       <c r="L76">
         <v>0</v>
       </c>
-      <c r="M76" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M76" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>67</v>
       </c>
       <c r="B77" t="s">
         <v>78</v>
       </c>
-      <c r="C77" s="5">
+      <c r="C77" s="4">
         <v>3.0499999999999999E-5</v>
       </c>
       <c r="D77">
@@ -4447,19 +4429,19 @@
       <c r="L77">
         <v>0</v>
       </c>
-      <c r="M77" s="7">
+      <c r="M77" s="6">
         <f t="shared" si="1"/>
         <v>3.1794926813960402E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>68</v>
       </c>
       <c r="B78" t="s">
         <v>79</v>
       </c>
-      <c r="C78" s="4">
+      <c r="C78" s="3">
         <v>0</v>
       </c>
       <c r="D78">
@@ -4489,19 +4471,19 @@
       <c r="L78">
         <v>0</v>
       </c>
-      <c r="M78" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M78" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>69</v>
       </c>
       <c r="B79" t="s">
         <v>80</v>
       </c>
-      <c r="C79" s="4">
+      <c r="C79" s="3">
         <v>0</v>
       </c>
       <c r="D79">
@@ -4531,19 +4513,19 @@
       <c r="L79">
         <v>0</v>
       </c>
-      <c r="M79" s="7">
+      <c r="M79" s="6">
         <f t="shared" si="1"/>
         <v>3.8669E-8</v>
       </c>
     </row>
-    <row r="80" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>70</v>
       </c>
       <c r="B80" t="s">
         <v>81</v>
       </c>
-      <c r="C80" s="4">
+      <c r="C80" s="3">
         <v>2.8068100000000002E-4</v>
       </c>
       <c r="D80">
@@ -4573,19 +4555,19 @@
       <c r="L80">
         <v>0</v>
       </c>
-      <c r="M80" s="7">
+      <c r="M80" s="6">
         <f t="shared" si="1"/>
         <v>1.8033490000000001E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>71</v>
       </c>
       <c r="B81" t="s">
         <v>82</v>
       </c>
-      <c r="C81" s="4">
+      <c r="C81" s="3">
         <v>0</v>
       </c>
       <c r="D81">
@@ -4615,19 +4597,19 @@
       <c r="L81">
         <v>0</v>
       </c>
-      <c r="M81" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M81" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>72</v>
       </c>
       <c r="B82" t="s">
         <v>83</v>
       </c>
-      <c r="C82" s="4">
+      <c r="C82" s="3">
         <v>0</v>
       </c>
       <c r="D82">
@@ -4657,19 +4639,19 @@
       <c r="L82">
         <v>0</v>
       </c>
-      <c r="M82" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M82" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>73</v>
       </c>
       <c r="B83" t="s">
         <v>84</v>
       </c>
-      <c r="C83" s="4">
+      <c r="C83" s="3">
         <v>0</v>
       </c>
       <c r="D83">
@@ -4699,19 +4681,19 @@
       <c r="L83">
         <v>0</v>
       </c>
-      <c r="M83" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M83" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>74</v>
       </c>
       <c r="B84" t="s">
         <v>85</v>
       </c>
-      <c r="C84" s="4">
+      <c r="C84" s="3">
         <v>0</v>
       </c>
       <c r="D84">
@@ -4741,19 +4723,19 @@
       <c r="L84">
         <v>0</v>
       </c>
-      <c r="M84" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M84" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>75</v>
       </c>
       <c r="B85" t="s">
         <v>86</v>
       </c>
-      <c r="C85" s="4">
+      <c r="C85" s="3">
         <v>0</v>
       </c>
       <c r="D85">
@@ -4783,19 +4765,19 @@
       <c r="L85">
         <v>0</v>
       </c>
-      <c r="M85" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M85" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>76</v>
       </c>
       <c r="B86" t="s">
         <v>87</v>
       </c>
-      <c r="C86" s="4">
+      <c r="C86" s="3">
         <v>0</v>
       </c>
       <c r="D86">
@@ -4825,19 +4807,19 @@
       <c r="L86">
         <v>0</v>
       </c>
-      <c r="M86" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M86" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>77</v>
       </c>
       <c r="B87" t="s">
         <v>88</v>
       </c>
-      <c r="C87" s="4">
+      <c r="C87" s="3">
         <v>0</v>
       </c>
       <c r="D87">
@@ -4867,19 +4849,19 @@
       <c r="L87">
         <v>0</v>
       </c>
-      <c r="M87" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M87" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>78</v>
       </c>
       <c r="B88" t="s">
         <v>89</v>
       </c>
-      <c r="C88" s="4">
+      <c r="C88" s="3">
         <v>0</v>
       </c>
       <c r="D88">
@@ -4909,19 +4891,19 @@
       <c r="L88">
         <v>0</v>
       </c>
-      <c r="M88" s="7">
-        <f t="shared" ref="M88:M98" si="2">SUM(C88:L88)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M88" s="6">
+        <f t="shared" ref="M88:M97" si="2">SUM(C88:L88)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>79</v>
       </c>
       <c r="B89" t="s">
         <v>90</v>
       </c>
-      <c r="C89" s="4">
+      <c r="C89" s="3">
         <v>0</v>
       </c>
       <c r="D89">
@@ -4951,19 +4933,19 @@
       <c r="L89">
         <v>0</v>
       </c>
-      <c r="M89" s="7">
+      <c r="M89" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>80</v>
       </c>
       <c r="B90" t="s">
         <v>91</v>
       </c>
-      <c r="C90" s="4">
+      <c r="C90" s="3">
         <v>0</v>
       </c>
       <c r="D90">
@@ -4993,19 +4975,19 @@
       <c r="L90">
         <v>0</v>
       </c>
-      <c r="M90" s="7">
+      <c r="M90" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>81</v>
       </c>
       <c r="B91" t="s">
         <v>92</v>
       </c>
-      <c r="C91" s="4">
+      <c r="C91" s="3">
         <v>0</v>
       </c>
       <c r="D91">
@@ -5035,19 +5017,19 @@
       <c r="L91">
         <v>0</v>
       </c>
-      <c r="M91" s="7">
+      <c r="M91" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>82</v>
       </c>
       <c r="B92" t="s">
         <v>93</v>
       </c>
-      <c r="C92" s="4">
+      <c r="C92" s="3">
         <v>0</v>
       </c>
       <c r="D92">
@@ -5077,19 +5059,19 @@
       <c r="L92">
         <v>0</v>
       </c>
-      <c r="M92" s="7">
+      <c r="M92" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>83</v>
       </c>
       <c r="B93" t="s">
         <v>94</v>
       </c>
-      <c r="C93" s="4">
+      <c r="C93" s="3">
         <v>0</v>
       </c>
       <c r="D93">
@@ -5119,19 +5101,19 @@
       <c r="L93">
         <v>0</v>
       </c>
-      <c r="M93" s="7">
+      <c r="M93" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>84</v>
       </c>
       <c r="B94" t="s">
         <v>95</v>
       </c>
-      <c r="C94" s="4">
+      <c r="C94" s="3">
         <v>0</v>
       </c>
       <c r="D94">
@@ -5161,19 +5143,19 @@
       <c r="L94">
         <v>0</v>
       </c>
-      <c r="M94" s="7">
+      <c r="M94" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>85</v>
       </c>
       <c r="B95" t="s">
         <v>96</v>
       </c>
-      <c r="C95" s="4">
+      <c r="C95" s="3">
         <v>0</v>
       </c>
       <c r="D95">
@@ -5203,19 +5185,19 @@
       <c r="L95">
         <v>0</v>
       </c>
-      <c r="M95" s="7">
+      <c r="M95" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>86</v>
       </c>
       <c r="B96" t="s">
         <v>97</v>
       </c>
-      <c r="C96" s="4">
+      <c r="C96" s="3">
         <v>0</v>
       </c>
       <c r="D96">
@@ -5245,19 +5227,19 @@
       <c r="L96">
         <v>0</v>
       </c>
-      <c r="M96" s="7">
+      <c r="M96" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>87</v>
       </c>
       <c r="B97" t="s">
         <v>98</v>
       </c>
-      <c r="C97" s="4">
+      <c r="C97" s="3">
         <v>0</v>
       </c>
       <c r="D97">
@@ -5287,73 +5269,65 @@
       <c r="L97">
         <v>0</v>
       </c>
-      <c r="M97" s="7">
+      <c r="M97" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
       <c r="B98" t="s">
         <v>99</v>
       </c>
-      <c r="C98" s="4">
+      <c r="C98" s="3">
         <f>SUM(C2:C97)</f>
         <v>4.5698270999999999E-3</v>
       </c>
-      <c r="D98" s="4">
+      <c r="D98" s="3">
         <f t="shared" ref="D98:M98" si="3">SUM(D2:D97)</f>
         <v>8.6906019775467219E-2</v>
       </c>
-      <c r="E98" s="4">
+      <c r="E98" s="3">
         <f t="shared" si="3"/>
         <v>0.69864092032885472</v>
       </c>
-      <c r="F98" s="4">
+      <c r="F98" s="3">
         <f t="shared" si="3"/>
         <v>4.1512039494141E-2</v>
       </c>
-      <c r="G98" s="4">
+      <c r="G98" s="3">
         <f t="shared" si="3"/>
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="H98" s="4">
+      <c r="H98" s="3">
         <f t="shared" si="3"/>
         <v>5.9224725600966636E-2</v>
       </c>
-      <c r="I98" s="4">
+      <c r="I98" s="3">
         <f t="shared" si="3"/>
         <v>0.7045120620310007</v>
       </c>
-      <c r="J98" s="4">
+      <c r="J98" s="3">
         <f t="shared" si="3"/>
         <v>4.9034589245621596E-2</v>
       </c>
-      <c r="K98" s="4">
+      <c r="K98" s="3">
         <f t="shared" si="3"/>
         <v>2.1227665976078377E-3</v>
       </c>
-      <c r="L98" s="4">
+      <c r="L98" s="3">
         <f t="shared" si="3"/>
         <v>0.40482419077952964</v>
       </c>
-      <c r="M98" s="4">
+      <c r="M98" s="3">
         <f t="shared" si="3"/>
         <v>2.0513571409531894</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M98" xr:uid="{A1B61ACA-ED6A-4045-8EF4-52A6AB899584}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Walleye pollock"/>
-        <filter val="Walleye pollock adult"/>
-        <filter val="Walleye pollock juvenile"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:M98" xr:uid="{A1B61ACA-ED6A-4045-8EF4-52A6AB899584}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5362,8 +5336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D707479-533E-40A4-A3E2-3B617A22A4E2}">
   <dimension ref="A1:M98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M63" sqref="M63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5373,42 +5347,42 @@
     <col min="3" max="13" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" t="s">
         <v>108</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" t="s">
         <v>109</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" t="s">
         <v>110</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" t="s">
         <v>111</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="M1" s="10" t="s">
+      <c r="H1" t="s">
+        <v>170</v>
+      </c>
+      <c r="I1" t="s">
+        <v>171</v>
+      </c>
+      <c r="J1" t="s">
+        <v>172</v>
+      </c>
+      <c r="K1" t="s">
+        <v>173</v>
+      </c>
+      <c r="L1" t="s">
+        <v>174</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>2</v>
       </c>
     </row>
@@ -5652,8 +5626,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="11" t="s">
+    <row r="22" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="9" t="s">
         <v>23</v>
       </c>
       <c r="M22"/>
@@ -5802,8 +5776,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="11" t="s">
+    <row r="35" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="9" t="s">
         <v>36</v>
       </c>
       <c r="M35"/>
@@ -5832,8 +5806,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="11" t="s">
+    <row r="38" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="9" t="s">
         <v>39</v>
       </c>
       <c r="M38"/>
@@ -5842,7 +5816,7 @@
       <c r="A39">
         <v>35</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="5" t="s">
         <v>40</v>
       </c>
       <c r="D39">
@@ -5868,8 +5842,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="11" t="s">
+    <row r="41" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="9" t="s">
         <v>42</v>
       </c>
       <c r="M41"/>
@@ -5878,7 +5852,7 @@
       <c r="A42">
         <v>37</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="5" t="s">
         <v>43</v>
       </c>
       <c r="M42">
@@ -5898,8 +5872,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="11" t="s">
+    <row r="44" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="9" t="s">
         <v>45</v>
       </c>
       <c r="M44"/>
@@ -5970,8 +5944,8 @@
         <v>5.6801366449573815E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="11" t="s">
+    <row r="49" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="9" t="s">
         <v>50</v>
       </c>
       <c r="M49"/>
@@ -6078,8 +6052,8 @@
         <v>9.8263967275634065E-4</v>
       </c>
     </row>
-    <row r="56" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="11" t="s">
+    <row r="56" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="9" t="s">
         <v>57</v>
       </c>
       <c r="M56"/>
@@ -6114,8 +6088,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="11" t="s">
+    <row r="59" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="9" t="s">
         <v>60</v>
       </c>
       <c r="M59"/>
@@ -6150,8 +6124,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="11" t="s">
+    <row r="62" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="9" t="s">
         <v>63</v>
       </c>
       <c r="M62"/>
@@ -6214,7 +6188,7 @@
       <c r="A67">
         <v>57</v>
       </c>
-      <c r="B67" s="6" t="s">
+      <c r="B67" s="5" t="s">
         <v>68</v>
       </c>
       <c r="E67">
@@ -6271,7 +6245,7 @@
       <c r="E71">
         <v>4.8899130634794168E-5</v>
       </c>
-      <c r="M71" s="8">
+      <c r="M71" s="7">
         <f t="shared" si="1"/>
         <v>4.8899130634794168E-5</v>
       </c>

</xml_diff>